<commit_message>
Generated BOM and CPL files
</commit_message>
<xml_diff>
--- a/cam/RP2040-Eins-20231121-JLCPCB-BOM-SOIC.xlsx
+++ b/cam/RP2040-Eins-20231121-JLCPCB-BOM-SOIC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AG\Documents\KiCad\7.0\projects\RP2040-Eins\cam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4BBE456-5748-49AF-83C7-9C0A236AC60A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03581ACC-13EF-4E2D-A75C-ED38F9612684}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="372" yWindow="1644" windowWidth="12336" windowHeight="18756" xr2:uid="{7B845E16-6401-438E-89AD-84A195B2B6BE}"/>
+    <workbookView xWindow="12156" yWindow="2460" windowWidth="12336" windowHeight="18756" xr2:uid="{7B845E16-6401-438E-89AD-84A195B2B6BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -79,9 +79,6 @@
     <t>2.2uF</t>
   </si>
   <si>
-    <t>R3,R2,R8,R9,R5,R4</t>
-  </si>
-  <si>
     <t>10k</t>
   </si>
   <si>
@@ -392,6 +389,9 @@
   </si>
   <si>
     <t>C106074</t>
+  </si>
+  <si>
+    <t>R3,R8,R9,R5,R4</t>
   </si>
 </sst>
 </file>
@@ -758,7 +758,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -772,7 +772,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -781,10 +781,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -798,7 +798,7 @@
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E2" t="s">
         <v>4</v>
@@ -812,10 +812,10 @@
         <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E3" t="s">
         <v>6</v>
@@ -829,13 +829,13 @@
         <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -846,10 +846,10 @@
         <v>8</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E5" t="s">
         <v>9</v>
@@ -857,19 +857,19 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E6" t="s">
         <v>10</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D6" t="s">
-        <v>72</v>
-      </c>
-      <c r="E6" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -877,16 +877,16 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E7" t="s">
         <v>12</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D7" t="s">
-        <v>69</v>
-      </c>
-      <c r="E7" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -894,16 +894,16 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
+        <v>98</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D8" t="s">
+        <v>97</v>
+      </c>
+      <c r="E8" t="s">
         <v>99</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="D8" t="s">
-        <v>98</v>
-      </c>
-      <c r="E8" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -911,16 +911,16 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D9" t="s">
+        <v>110</v>
+      </c>
+      <c r="E9" t="s">
         <v>14</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="D9" t="s">
-        <v>111</v>
-      </c>
-      <c r="E9" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -928,16 +928,16 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D10" t="s">
+        <v>103</v>
+      </c>
+      <c r="E10" t="s">
         <v>16</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="D10" t="s">
-        <v>104</v>
-      </c>
-      <c r="E10" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -945,16 +945,16 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" t="s">
+        <v>72</v>
+      </c>
+      <c r="E11" t="s">
         <v>18</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D11" t="s">
-        <v>73</v>
-      </c>
-      <c r="E11" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -962,16 +962,16 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D12" t="s">
+        <v>91</v>
+      </c>
+      <c r="E12" t="s">
         <v>20</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D12" t="s">
-        <v>92</v>
-      </c>
-      <c r="E12" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -979,16 +979,16 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -996,16 +996,16 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D14" t="s">
+        <v>73</v>
+      </c>
+      <c r="E14" t="s">
         <v>23</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D14" t="s">
-        <v>74</v>
-      </c>
-      <c r="E14" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -1013,16 +1013,16 @@
         <v>11</v>
       </c>
       <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" t="s">
+        <v>79</v>
+      </c>
+      <c r="E15" t="s">
         <v>25</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D15" t="s">
-        <v>80</v>
-      </c>
-      <c r="E15" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -1030,16 +1030,16 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D16" t="s">
+        <v>87</v>
+      </c>
+      <c r="E16" t="s">
         <v>27</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D16" t="s">
-        <v>88</v>
-      </c>
-      <c r="E16" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -1047,16 +1047,16 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D17" t="s">
+        <v>76</v>
+      </c>
+      <c r="E17" t="s">
         <v>29</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D17" t="s">
-        <v>77</v>
-      </c>
-      <c r="E17" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -1064,16 +1064,16 @@
         <v>2</v>
       </c>
       <c r="B18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D18" t="s">
+        <v>95</v>
+      </c>
+      <c r="E18" t="s">
         <v>31</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D18" t="s">
-        <v>96</v>
-      </c>
-      <c r="E18" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -1081,16 +1081,16 @@
         <v>2</v>
       </c>
       <c r="B19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D19" t="s">
+        <v>66</v>
+      </c>
+      <c r="E19" t="s">
         <v>33</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D19" t="s">
-        <v>67</v>
-      </c>
-      <c r="E19" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -1098,16 +1098,16 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D20" t="s">
+        <v>105</v>
+      </c>
+      <c r="E20" t="s">
         <v>35</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="D20" t="s">
-        <v>106</v>
-      </c>
-      <c r="E20" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -1115,16 +1115,16 @@
         <v>4</v>
       </c>
       <c r="B21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C21" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D21" t="s">
         <v>81</v>
       </c>
-      <c r="D21" t="s">
-        <v>82</v>
-      </c>
       <c r="E21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -1132,16 +1132,16 @@
         <v>1</v>
       </c>
       <c r="B22" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D22" t="s">
+        <v>107</v>
+      </c>
+      <c r="E22" t="s">
         <v>38</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="D22" t="s">
-        <v>108</v>
-      </c>
-      <c r="E22" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -1149,16 +1149,16 @@
         <v>1</v>
       </c>
       <c r="B23" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D23" t="s">
+        <v>106</v>
+      </c>
+      <c r="E23" t="s">
         <v>40</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="D23" t="s">
-        <v>107</v>
-      </c>
-      <c r="E23" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -1166,16 +1166,16 @@
         <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C24" t="s">
+        <v>77</v>
+      </c>
+      <c r="D24" t="s">
+        <v>112</v>
+      </c>
+      <c r="E24" t="s">
         <v>78</v>
-      </c>
-      <c r="D24" t="s">
-        <v>113</v>
-      </c>
-      <c r="E24" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -1183,16 +1183,16 @@
         <v>1</v>
       </c>
       <c r="B25" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D25" t="s">
+        <v>82</v>
+      </c>
+      <c r="E25" t="s">
         <v>43</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D25" t="s">
-        <v>83</v>
-      </c>
-      <c r="E25" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -1200,16 +1200,16 @@
         <v>1</v>
       </c>
       <c r="B26" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D26" t="s">
+        <v>101</v>
+      </c>
+      <c r="E26" t="s">
         <v>45</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="D26" t="s">
-        <v>102</v>
-      </c>
-      <c r="E26" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -1217,16 +1217,16 @@
         <v>1</v>
       </c>
       <c r="B27" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D27" t="s">
+        <v>89</v>
+      </c>
+      <c r="E27" t="s">
         <v>47</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="D27" t="s">
-        <v>90</v>
-      </c>
-      <c r="E27" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -1234,16 +1234,16 @@
         <v>1</v>
       </c>
       <c r="B28" t="s">
+        <v>48</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D28" t="s">
+        <v>113</v>
+      </c>
+      <c r="E28" t="s">
         <v>49</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D28" t="s">
-        <v>114</v>
-      </c>
-      <c r="E28" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
@@ -1251,16 +1251,16 @@
         <v>1</v>
       </c>
       <c r="B29" t="s">
+        <v>50</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="D29" t="s">
+        <v>94</v>
+      </c>
+      <c r="E29" t="s">
         <v>52</v>
-      </c>
-      <c r="D29" t="s">
-        <v>95</v>
-      </c>
-      <c r="E29" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
@@ -1268,16 +1268,16 @@
         <v>1</v>
       </c>
       <c r="B30" t="s">
+        <v>53</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D30" t="s">
+        <v>105</v>
+      </c>
+      <c r="E30" t="s">
         <v>54</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="D30" t="s">
-        <v>106</v>
-      </c>
-      <c r="E30" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
@@ -1285,16 +1285,16 @@
         <v>1</v>
       </c>
       <c r="B31" t="s">
+        <v>55</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D31" t="s">
+        <v>108</v>
+      </c>
+      <c r="E31" t="s">
         <v>56</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D31" t="s">
-        <v>109</v>
-      </c>
-      <c r="E31" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
@@ -1302,16 +1302,16 @@
         <v>1</v>
       </c>
       <c r="B32" t="s">
+        <v>57</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D32" t="s">
+        <v>111</v>
+      </c>
+      <c r="E32" t="s">
         <v>58</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="D32" t="s">
-        <v>112</v>
-      </c>
-      <c r="E32" t="s">
-        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>